<commit_message>
UPDATE: Nama dosen pada select disusun secara ascending A samapi Z
</commit_message>
<xml_diff>
--- a/uploads/jadwal-dosen2.xlsx
+++ b/uploads/jadwal-dosen2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS TUF GAMING\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C7481B-DB57-400A-AC1A-23A29A94E73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E50B033-0353-44A7-9B8F-FCF21594DC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A3982EF8-5654-4D17-B35A-D4535971505A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
   <si>
     <t>08:00-10:30</t>
   </si>
@@ -81,9 +81,6 @@
     <t>FADLISYAH, S.Si.,MT</t>
   </si>
   <si>
-    <t>CUT AGUSNIAR, S.T., M.Cs, LIDYA ROSNITA, S.T., M. Kom</t>
-  </si>
-  <si>
     <t>RIZAL, S.Si, M.IT</t>
   </si>
   <si>
@@ -106,6 +103,12 @@
   </si>
   <si>
     <t>10:30-13:10</t>
+  </si>
+  <si>
+    <t>CUT AGUSNIAR, S.T., M.Cs</t>
+  </si>
+  <si>
+    <t>LIDYA ROSNITA, S.T., M. Kom</t>
   </si>
 </sst>
 </file>
@@ -129,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -152,13 +155,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -475,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D213A8B6-5EDA-4FF4-AC64-4EB77E26D40E}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,7 +534,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -529,7 +546,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -541,7 +558,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -554,7 +571,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -566,7 +583,7 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -617,7 +634,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -653,7 +670,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -713,7 +730,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -742,22 +759,26 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="D22" s="1" t="s">
         <v>0</v>
       </c>
@@ -766,7 +787,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -778,19 +799,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -802,7 +823,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -812,6 +833,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>